<commit_message>
Generated the file for CustomerGreylock Federal Credit Union - HQ @ 75 Kellogg in the production server
</commit_message>
<xml_diff>
--- a/Greylock Federal Credit Union - HQ @ 75 Kellogg.xlsx
+++ b/Greylock Federal Credit Union - HQ @ 75 Kellogg.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="VMware" sheetId="1" r:id="rId1"/>
     <sheet name="Network Device" sheetId="2" r:id="rId2"/>
+    <sheet name="Server" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="121">
   <si>
     <t>Greylock Federal Credit Union - HQ @ 75 Kellogg</t>
   </si>
@@ -542,6 +543,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>273797</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>100080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2102597" cy="481080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:J19" totalsRowCount="1">
   <autoFilter ref="A5:J18"/>
@@ -564,6 +608,28 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A5:M17" totalsRowCount="1">
   <autoFilter ref="A5:M16"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="5" name="Column5"/>
+    <tableColumn id="6" name="Column6"/>
+    <tableColumn id="7" name="Column7"/>
+    <tableColumn id="8" name="Column8"/>
+    <tableColumn id="9" name="Column9"/>
+    <tableColumn id="10" name="Column10"/>
+    <tableColumn id="11" name="Column11"/>
+    <tableColumn id="12" name="Column12"/>
+    <tableColumn id="13" name="Column13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:M12" totalsRowCount="1">
+  <autoFilter ref="A5:M11"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1877,4 +1943,83 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" t="s">
+        <v>106</v>
+      </c>
+      <c r="L5" t="s">
+        <v>107</v>
+      </c>
+      <c r="M5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:M3"/>
+    <mergeCell ref="A4:M4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>